<commit_message>
Updated FindUserById to eager load all related entitites
</commit_message>
<xml_diff>
--- a/EmailConfirmationServer/Files/TestSheet2.xlsx
+++ b/EmailConfirmationServer/Files/TestSheet2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\izmac\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEBC58FB-2F1C-48C1-A065-E329B5F97DE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8BFD700-09C0-4D4F-BBA1-899CCBED793D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{227B31AE-315F-4CFF-8A71-775C54A0AB13}"/>
   </bookViews>
@@ -69,10 +69,10 @@
     <t>Crazy</t>
   </si>
   <si>
-    <t>Z</t>
-  </si>
-  <si>
-    <t>Man</t>
+    <t>Zman</t>
+  </si>
+  <si>
+    <t>Zach</t>
   </si>
 </sst>
 </file>
@@ -452,7 +452,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>